<commit_message>
Commit completo prima dell'attivazione delle sessioni evento
</commit_message>
<xml_diff>
--- a/public/users.xlsx
+++ b/public/users.xlsx
@@ -139,7 +139,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -162,19 +162,39 @@
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Organization</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Gender</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Sectors</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
           <t>Groups</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>Business name</t>
         </is>
       </c>
     </row>
     <row collapsed="" customFormat="false" customHeight="" hidden="" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>Greco Roberto</t>
+          <t>Roberto Greco</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -184,10 +204,36 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>international and intergovernmental organizations</t>
-        </is>
-      </c>
-      <c r="D2" s="3"/>
+          <t>Italy</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>Square</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
+        <is>
+          <t>31-50</t>
+        </is>
+      </c>
+      <c r="F2" s="3" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>other
+IT</t>
+        </is>
+      </c>
+      <c r="H2" s="3" t="inlineStr">
+        <is>
+          <t>other
+information</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>